<commit_message>
User data 3.0 to dev
</commit_message>
<xml_diff>
--- a/user-data/fragile-states/fragile-states.xlsx
+++ b/user-data/fragile-states/fragile-states.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="540">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -1598,19 +1598,10 @@
     <t xml:space="preserve">Description: Fragile states categories.</t>
   </si>
   <si>
-    <t xml:space="preserve">Description: NA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Units of measure: index</t>
   </si>
   <si>
-    <t xml:space="preserve">Units of measure: NA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Source: Development Initiatives based on Fund for Peace Fragile States Index.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source: DI</t>
   </si>
   <si>
     <t xml:space="preserve">Notes:</t>
@@ -1996,25 +1987,25 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>529</v>
-      </c>
+      <c r="A5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
+    <row r="9">
+      <c r="A9" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8"/>
-    </row>
-    <row r="9">
-      <c r="A9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -2022,74 +2013,53 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11"/>
+      <c r="A11" t="s">
+        <v>533</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12"/>
+      <c r="A12" t="s">
+        <v>531</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
         <v>539</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "User data 3.0"
This reverts commit 9634c02944bc8d829eda4399a706e0a20ee28b44.
</commit_message>
<xml_diff>
--- a/user-data/fragile-states/fragile-states.xlsx
+++ b/user-data/fragile-states/fragile-states.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="543">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -1598,10 +1598,19 @@
     <t xml:space="preserve">Description: Fragile states categories.</t>
   </si>
   <si>
+    <t xml:space="preserve">Description: NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Units of measure: index</t>
   </si>
   <si>
+    <t xml:space="preserve">Units of measure: NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Source: Development Initiatives based on Fund for Peace Fragile States Index.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: DI</t>
   </si>
   <si>
     <t xml:space="preserve">Notes:</t>
@@ -1987,25 +1996,25 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5"/>
+      <c r="A5" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7"/>
+      <c r="A7" t="s">
+        <v>531</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>530</v>
-      </c>
+      <c r="A8"/>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>531</v>
-      </c>
+      <c r="A9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -2013,53 +2022,74 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>533</v>
-      </c>
+      <c r="A11"/>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>531</v>
-      </c>
+      <c r="A12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
         <v>539</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>